<commit_message>
Final adjustments for JCON Europe
</commit_message>
<xml_diff>
--- a/talk-schedule.xlsx
+++ b/talk-schedule.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanno/Code/talks/slide-decks/from-zero-to-secured/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62108303-2957-684A-B788-0325AD824E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE57BD8A-B282-2040-B849-07E64C47F73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{A27474F1-0DB6-C54B-BE04-0E23ACC02F33}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="21580" xr2:uid="{A27474F1-0DB6-C54B-BE04-0E23ACC02F33}"/>
   </bookViews>
   <sheets>
     <sheet name="45m" sheetId="2" r:id="rId1"/>
     <sheet name="90m" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -133,6 +133,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -228,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -237,30 +240,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="45" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="45" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="45" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,77 +599,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA13031B-B79E-794B-AA4E-843A15820FA1}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="248" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="6" hidden="1" customWidth="1"/>
     <col min="7" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="10"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -675,24 +681,23 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6">
+      <c r="F3" s="4"/>
+      <c r="G3" s="5">
         <v>0</v>
       </c>
-      <c r="H3" s="6">
-        <f>G3+D3+F3</f>
-        <v>1.3888888888888889E-3</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="H3" s="5">
+        <v>1.736111111111111E-3</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -702,26 +707,24 @@
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6">
+      <c r="F4" s="4"/>
+      <c r="G4" s="5">
         <f>H3</f>
-        <v>1.3888888888888889E-3</v>
-      </c>
-      <c r="H4" s="6">
-        <f>G4+D4+F4</f>
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="I4" s="6">
-        <f>J3</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10">
+        <v>1.736111111111111E-3</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -731,26 +734,24 @@
       <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>3.4722222222222224E-4</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6">
-        <f t="shared" ref="G5:I15" si="0">H4</f>
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="H5" s="6">
-        <f t="shared" ref="H5:H15" si="1">G5+D5+F5</f>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5">
+        <f t="shared" ref="G5:G15" si="0">H4</f>
         <v>3.1250000000000002E-3</v>
       </c>
-      <c r="I5" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="H5" s="5">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -760,30 +761,28 @@
       <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="G6" s="6">
-        <f t="shared" si="0"/>
-        <v>3.1250000000000002E-3</v>
-      </c>
-      <c r="H6" s="6">
-        <f t="shared" si="1"/>
-        <v>5.5555555555555558E-3</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="H6" s="5">
+        <v>6.5972222222222222E-3</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -793,26 +792,24 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>2.4305555555555556E-3</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6">
-        <f t="shared" si="0"/>
-        <v>5.5555555555555558E-3</v>
-      </c>
-      <c r="H7" s="6">
-        <f t="shared" si="1"/>
-        <v>7.9861111111111105E-3</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="F7" s="4"/>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>6.5972222222222222E-3</v>
+      </c>
+      <c r="H7" s="5">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -822,30 +819,28 @@
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>3.8194444444444443E-3</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="G8" s="6">
-        <f t="shared" si="0"/>
-        <v>7.9861111111111105E-3</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="1"/>
-        <v>1.3194444444444444E-2</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -855,30 +850,28 @@
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>3.8194444444444443E-3</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="G9" s="6">
-        <f t="shared" si="0"/>
-        <v>1.3194444444444444E-2</v>
-      </c>
-      <c r="H9" s="6">
-        <f t="shared" si="1"/>
-        <v>1.7708333333333333E-2</v>
-      </c>
-      <c r="I9" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1.6319444444444445E-2</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -888,26 +881,24 @@
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>1.0416666666666667E-3</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6">
-        <f t="shared" si="0"/>
-        <v>1.7708333333333333E-2</v>
-      </c>
-      <c r="H10" s="6">
-        <f t="shared" si="1"/>
-        <v>1.8749999999999999E-2</v>
-      </c>
-      <c r="I10" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="F10" s="4"/>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>1.6319444444444445E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1.8055555555555554E-2</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -917,30 +908,28 @@
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>1.8749999999999999E-2</v>
-      </c>
-      <c r="H11" s="6">
-        <f t="shared" si="1"/>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8055555555555554E-2</v>
+      </c>
+      <c r="H11" s="5">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="I11" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -950,26 +939,24 @@
       <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6">
+      <c r="F12" s="4"/>
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="H12" s="6">
-        <f t="shared" si="1"/>
-        <v>2.2916666666666665E-2</v>
-      </c>
-      <c r="I12" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="H12" s="5">
+        <v>2.2569444444444444E-2</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -979,30 +966,28 @@
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>3.8194444444444443E-3</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="G13" s="6">
-        <f t="shared" si="0"/>
-        <v>2.2916666666666665E-2</v>
-      </c>
-      <c r="H13" s="6">
-        <f t="shared" si="1"/>
-        <v>2.8124999999999997E-2</v>
-      </c>
-      <c r="I13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>2.2569444444444444E-2</v>
+      </c>
+      <c r="H13" s="5">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1012,26 +997,24 @@
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>2.8124999999999997E-2</v>
-      </c>
-      <c r="H14" s="6">
-        <f t="shared" si="1"/>
-        <v>3.020833333333333E-2</v>
-      </c>
-      <c r="I14" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="F14" s="4"/>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="H14" s="5">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1041,24 +1024,22 @@
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>1.0416666666666667E-3</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>3.020833333333333E-2</v>
-      </c>
-      <c r="H15" s="6">
-        <f t="shared" si="1"/>
-        <v>3.1249999999999997E-2</v>
-      </c>
-      <c r="I15" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="6"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="H15" s="5">
+        <v>3.125E-2</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1069,10 +1050,31 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="K3:K15">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="H4:H15" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1096,44 +1098,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="11" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
@@ -1145,15 +1147,15 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6">
+      <c r="F3" s="4"/>
+      <c r="G3" s="5">
         <v>0</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>G3+D3+F3</f>
         <v>4.8611111111111112E-3</v>
       </c>
@@ -1168,16 +1170,16 @@
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1.736111111111111E-3</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6">
+      <c r="F4" s="4"/>
+      <c r="G4" s="5">
         <f>H3</f>
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f>G4+D4+F4</f>
         <v>6.5972222222222222E-3</v>
       </c>
@@ -1192,20 +1194,20 @@
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>2.4305555555555556E-3</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f t="shared" ref="G5:G15" si="0">H4</f>
         <v>6.5972222222222222E-3</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f t="shared" ref="H5:H15" si="1">G5+D5+F5</f>
         <v>9.7222222222222206E-3</v>
       </c>
@@ -1220,20 +1222,20 @@
       <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>9.7222222222222224E-3</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>4.5138888888888885E-3</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>9.7222222222222206E-3</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f t="shared" si="1"/>
         <v>2.3958333333333331E-2</v>
       </c>
@@ -1248,20 +1250,20 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>4.5138888888888885E-3</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>2.3958333333333331E-2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" si="1"/>
         <v>2.9166666666666664E-2</v>
       </c>
@@ -1276,20 +1278,20 @@
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>2.9166666666666664E-2</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="1"/>
         <v>3.5763888888888887E-2</v>
       </c>
@@ -1304,20 +1306,20 @@
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>4.5138888888888885E-3</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>3.5763888888888887E-2</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="1"/>
         <v>4.0972222222222215E-2</v>
       </c>
@@ -1332,20 +1334,20 @@
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>2.7777777777777779E-3</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>4.0972222222222215E-2</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <f t="shared" si="1"/>
         <v>4.4097222222222211E-2</v>
       </c>
@@ -1360,20 +1362,20 @@
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>2.7777777777777779E-3</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>1.0416666666666667E-3</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f t="shared" si="0"/>
         <v>4.4097222222222211E-2</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <f t="shared" si="1"/>
         <v>4.7916666666666656E-2</v>
       </c>
@@ -1388,16 +1390,16 @@
       <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>1.736111111111111E-3</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="7">
+      <c r="F12" s="4"/>
+      <c r="G12" s="6">
         <f t="shared" si="0"/>
         <v>4.7916666666666656E-2</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <f t="shared" si="1"/>
         <v>4.9652777777777768E-2</v>
       </c>
@@ -1412,20 +1414,20 @@
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>5.208333333333333E-3</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <f t="shared" si="0"/>
         <v>4.9652777777777768E-2</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <f t="shared" si="1"/>
         <v>5.6944444444444436E-2</v>
       </c>
@@ -1440,16 +1442,16 @@
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>4.1666666666666666E-3</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7">
+      <c r="F14" s="4"/>
+      <c r="G14" s="6">
         <f t="shared" si="0"/>
         <v>5.6944444444444436E-2</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <f t="shared" si="1"/>
         <v>6.1111111111111102E-2</v>
       </c>
@@ -1464,28 +1466,28 @@
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="7">
+      <c r="F15" s="4"/>
+      <c r="G15" s="6">
         <f t="shared" si="0"/>
         <v>6.1111111111111102E-2</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <f t="shared" si="1"/>
         <v>6.2499999999999993E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>